<commit_message>
Add new approach pretrained models and related resources
</commit_message>
<xml_diff>
--- a/Kaggle-Competitions/Humpback Whale Detection Challenge/Approaches/Approaches and related resources.xlsx
+++ b/Kaggle-Competitions/Humpback Whale Detection Challenge/Approaches/Approaches and related resources.xlsx
@@ -1,13 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{47DF3F8C-A37B-4F76-B260-A04CFE7AF39B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="List of pretrained models Keras" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,12 +20,129 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
+  <si>
+    <t>Approach</t>
+  </si>
+  <si>
+    <t>S.No</t>
+  </si>
+  <si>
+    <t>Input Size</t>
+  </si>
+  <si>
+    <t>Ouput Size</t>
+  </si>
+  <si>
+    <t>Reference Link</t>
+  </si>
+  <si>
+    <t>https://keras.io/applications/</t>
+  </si>
+  <si>
+    <t>299 x 299</t>
+  </si>
+  <si>
+    <t>Model name</t>
+  </si>
+  <si>
+    <t>Xception</t>
+  </si>
+  <si>
+    <t>1000 Classes</t>
+  </si>
+  <si>
+    <t>VGG 16</t>
+  </si>
+  <si>
+    <t>224 x 224</t>
+  </si>
+  <si>
+    <t>Pretrained Dataset</t>
+  </si>
+  <si>
+    <t>ImageNet</t>
+  </si>
+  <si>
+    <t>VGG 19</t>
+  </si>
+  <si>
+    <t>ResNet50</t>
+  </si>
+  <si>
+    <t>Inception V3</t>
+  </si>
+  <si>
+    <t>Inception ResNetV2</t>
+  </si>
+  <si>
+    <t>MobileNet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">224 x 224 </t>
+  </si>
+  <si>
+    <t>DenseNet</t>
+  </si>
+  <si>
+    <t>NASNetMobile</t>
+  </si>
+  <si>
+    <t>NASNetLarge</t>
+  </si>
+  <si>
+    <t>331 x 331</t>
+  </si>
+  <si>
+    <t>MobileNetV2</t>
+  </si>
+  <si>
+    <t>Library</t>
+  </si>
+  <si>
+    <t>Keras</t>
+  </si>
+  <si>
+    <t>Pretrained Models</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Click Here</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -37,7 +156,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,14 +164,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -330,13 +470,291 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" location="'List of pretrained models Keras'!A1" display="Click Here" xr:uid="{ECA05357-FEAA-45FD-A722-845948354D6E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E0E2160-4451-42F1-A1DE-51539BA491A3}">
+  <dimension ref="A2:E27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C27" r:id="rId1" xr:uid="{C02DF66B-58BD-4742-9FBF-CEA631E24053}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add the issue and resolution for pretrained models
</commit_message>
<xml_diff>
--- a/Kaggle-Competitions/Humpback Whale Detection Challenge/Approaches/Approaches and related resources.xlsx
+++ b/Kaggle-Competitions/Humpback Whale Detection Challenge/Approaches/Approaches and related resources.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{47DF3F8C-A37B-4F76-B260-A04CFE7AF39B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{66363A7C-CA86-4B9C-B059-91F362761DDC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
   <si>
     <t>Approach</t>
   </si>
@@ -111,6 +111,18 @@
   </si>
   <si>
     <t>Click Here</t>
+  </si>
+  <si>
+    <t>Issue</t>
+  </si>
+  <si>
+    <t>Not able to download the weights using the command used in Keras website</t>
+  </si>
+  <si>
+    <t>Resolving method</t>
+  </si>
+  <si>
+    <t>The pretrained model weights are downloaded to the kaggle kernel</t>
   </si>
 </sst>
 </file>
@@ -471,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,9 +494,11 @@
     <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="70.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -497,8 +511,14 @@
       <c r="D1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -510,6 +530,12 @@
       </c>
       <c r="D2" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>